<commit_message>
feat: add edge 0-shot
</commit_message>
<xml_diff>
--- a/experiments/node/few_shot/nodes_0shot_0/ans.xlsx
+++ b/experiments/node/few_shot/nodes_0shot_0/ans.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qinsz\Desktop\NLP_project\03code\IDExtraction\experiments\node\few_shot\nodes_0shot_0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB63829F-23A7-4663-A8BB-E3D683FF7DE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56A2AFBF-7B73-4955-B285-E78687269C98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-5355" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1366,10 +1366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I105"/>
+  <dimension ref="A1:I107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="B105" sqref="B105:F105"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -4412,6 +4412,50 @@
         <v>0.89158576051779947</v>
       </c>
     </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B106">
+        <f>_xlfn.STDEV.S(B2:B104)</f>
+        <v>0.20218395799215896</v>
+      </c>
+      <c r="C106">
+        <f t="shared" ref="C106:F106" si="1">_xlfn.STDEV.S(C2:C104)</f>
+        <v>0.2133319067674016</v>
+      </c>
+      <c r="D106">
+        <f t="shared" si="1"/>
+        <v>0.28908757507272426</v>
+      </c>
+      <c r="E106">
+        <f t="shared" si="1"/>
+        <v>0.23382425941842236</v>
+      </c>
+      <c r="F106">
+        <f t="shared" si="1"/>
+        <v>0.22104517261309761</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B107">
+        <f>B106/SQRT(103)*1.96</f>
+        <v>3.9046683583423496E-2</v>
+      </c>
+      <c r="C107">
+        <f t="shared" ref="C107:F107" si="2">C106/SQRT(103)*1.96</f>
+        <v>4.119962604608908E-2</v>
+      </c>
+      <c r="D107">
+        <f t="shared" si="2"/>
+        <v>5.582990452784397E-2</v>
+      </c>
+      <c r="E107">
+        <f t="shared" si="2"/>
+        <v>4.5157202195010689E-2</v>
+      </c>
+      <c r="F107">
+        <f t="shared" si="2"/>
+        <v>4.2689246953022751E-2</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>